<commit_message>
Add labels after new language --INTEGRATION
</commit_message>
<xml_diff>
--- a/uploads/writeTemplate.xlsx
+++ b/uploads/writeTemplate.xlsx
@@ -4,82 +4,35 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="1 dashboard" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="2 signup" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="3 homePage" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="1 Us-en" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Label_id</t>
+  </si>
   <si>
     <t>Label_name</t>
   </si>
   <si>
-    <t>Label_value</t>
+    <t>Translation_value</t>
   </si>
   <si>
-    <t>Language_id</t>
+    <t>demoLabel1</t>
   </si>
   <si>
-    <t>userDatabase</t>
-  </si>
-  <si>
-    <t>logout</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>newLanguage</t>
-  </si>
-  <si>
-    <t>newPage</t>
-  </si>
-  <si>
-    <t>newLabel</t>
-  </si>
-  <si>
-    <t>updateLabel</t>
-  </si>
-  <si>
-    <t>fullTemplate</t>
-  </si>
-  <si>
-    <t>downloadTemplates</t>
-  </si>
-  <si>
-    <t>completeUpload</t>
-  </si>
-  <si>
-    <t>signUp</t>
-  </si>
-  <si>
-    <t>userName</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>email</t>
+    <t>demoLabel2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -87,22 +40,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <family val="4"/>
-      <sz val="15"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="#B0E0E6"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,10 +61,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,189 +402,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="3" width="28" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="C10:C500">
-      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C500">
-      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="3" width="28" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="C10:C500">
-      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C500">
-      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="3" width="28" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="C10:C500">
-      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C500">
-      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add labels after adding new page --INTEGRATION
</commit_message>
<xml_diff>
--- a/uploads/writeTemplate.xlsx
+++ b/uploads/writeTemplate.xlsx
@@ -4,28 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="1 Us-en" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Add_Labels" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Label_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Label_name</t>
   </si>
   <si>
-    <t>Translation_value</t>
+    <t>1 US-en</t>
   </si>
   <si>
-    <t>demoLabel1</t>
-  </si>
-  <si>
-    <t>demoLabel2</t>
+    <t>2 IN-hi</t>
   </si>
 </sst>
 </file>
@@ -402,11 +396,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="3" width="28" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -420,22 +414,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Fix errors in update template after merge
</commit_message>
<xml_diff>
--- a/uploads/writeTemplate.xlsx
+++ b/uploads/writeTemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>Translation_id</t>
   </si>
@@ -26,6 +26,33 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>hello english</t>
+  </si>
+  <si>
+    <t>US-en English</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>kannada hello</t>
+  </si>
+  <si>
+    <t>IN-kn Kannada</t>
+  </si>
+  <si>
+    <t>bye</t>
+  </si>
+  <si>
+    <t>hello in english</t>
+  </si>
+  <si>
+    <t>bye in english</t>
   </si>
 </sst>
 </file>
@@ -402,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -427,6 +454,108 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
query to fetch translations based on page and language completed
</commit_message>
<xml_diff>
--- a/uploads/writeTemplate.xlsx
+++ b/uploads/writeTemplate.xlsx
@@ -4,55 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Update_Labels" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Add_Labels" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
-  <si>
-    <t>Translation_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Label_name</t>
   </si>
   <si>
-    <t>Translation_value</t>
+    <t>1 US-en</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>hello english</t>
-  </si>
-  <si>
-    <t>US-en English</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>kannada hello</t>
-  </si>
-  <si>
-    <t>IN-kn Kannada</t>
-  </si>
-  <si>
-    <t>bye</t>
-  </si>
-  <si>
-    <t>hello in english</t>
-  </si>
-  <si>
-    <t>bye in english</t>
+    <t>2 IN-kn</t>
   </si>
 </sst>
 </file>
@@ -429,15 +396,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,114 +413,6 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>